<commit_message>
Added a new diagnostic column to the output csv: field in the destination document
</commit_message>
<xml_diff>
--- a/doc/crosswalk_rdmp.xlsx
+++ b/doc/crosswalk_rdmp.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Desktop/Provisioner/rb2-migrate/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D4053B-56EF-DA42-AA00-DF00CB37089E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C43031-1BD5-BB4B-B3E4-9AC5469C5D32}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22480" yWindow="-1500" windowWidth="27640" windowHeight="16540" xr2:uid="{D40799DA-BD77-124F-A81D-CFE600731E6F}"/>
+    <workbookView xWindow="-28820" yWindow="-1500" windowWidth="27640" windowHeight="16540" xr2:uid="{D40799DA-BD77-124F-A81D-CFE600731E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$90</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="139">
   <si>
     <t xml:space="preserve">Field </t>
   </si>
@@ -403,6 +406,45 @@
   </si>
   <si>
     <t>vivo:Dataset.redbox:MetadataStandard</t>
+  </si>
+  <si>
+    <t>locrel:clb.foaf:Person.1.person.dc:identifier</t>
+  </si>
+  <si>
+    <t>locrel:clb.foaf:Person.1.person.foaf:title</t>
+  </si>
+  <si>
+    <t>locrel:clb.foaf:Person.1.person.foaf:givenName</t>
+  </si>
+  <si>
+    <t>locrel:clb.foaf:Person.1.person.foaf:email</t>
+  </si>
+  <si>
+    <t>locrel:clb.foaf:Person.1.person.foaf:familyName</t>
+  </si>
+  <si>
+    <t>records</t>
+  </si>
+  <si>
+    <t>ethics_note</t>
+  </si>
+  <si>
+    <t>sensitivities</t>
+  </si>
+  <si>
+    <t>Existing</t>
+  </si>
+  <si>
+    <t>agls:policy_dc:identifier</t>
+  </si>
+  <si>
+    <t>agls:policy_skos:note</t>
+  </si>
+  <si>
+    <t>agls:protectiveMarking_dc:type</t>
+  </si>
+  <si>
+    <t>agls:protectiveMarking_skos:note</t>
   </si>
 </sst>
 </file>
@@ -754,19 +796,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0153FD-7F44-7F45-A0A3-8BCD7A703616}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -777,13 +821,16 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -791,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -802,13 +849,16 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" t="s">
         <v>116</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -818,8 +868,14 @@
       <c r="C4">
         <v>30</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -829,11 +885,17 @@
       <c r="C5">
         <v>52</v>
       </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
       <c r="E5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -843,8 +905,11 @@
       <c r="C6">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -855,7 +920,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -863,7 +928,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -871,7 +936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -881,11 +946,11 @@
       <c r="C10">
         <v>206</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -893,7 +958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -901,7 +966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -909,7 +974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -917,7 +982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -925,7 +990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -933,7 +998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -941,7 +1006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -952,7 +1017,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -963,7 +1028,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -974,29 +1039,29 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>34</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1004,7 +1069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>37</v>
       </c>
@@ -1014,11 +1079,11 @@
       <c r="C24">
         <v>0</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1028,22 +1093,22 @@
       <c r="C25">
         <v>0</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>40</v>
       </c>
       <c r="B26" t="s">
         <v>41</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1054,7 +1119,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1064,11 +1129,11 @@
       <c r="C28">
         <v>127</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1076,18 +1141,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>45</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1095,526 +1160,564 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>51</v>
       </c>
-      <c r="B32" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B37" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>49</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B38" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>47</v>
       </c>
-      <c r="B34" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="B39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>53</v>
       </c>
-      <c r="B35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B40" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>54</v>
       </c>
-      <c r="B36" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B41" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>55</v>
       </c>
-      <c r="B37" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B42" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>56</v>
       </c>
-      <c r="B38" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B43" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>57</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B44" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>58</v>
       </c>
-      <c r="B40" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B45" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>59</v>
       </c>
-      <c r="B41" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B46" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>60</v>
       </c>
-      <c r="B42" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B47" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>61</v>
       </c>
-      <c r="B43" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="B48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>62</v>
       </c>
-      <c r="B44" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="B49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>63</v>
       </c>
-      <c r="B45" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>64</v>
       </c>
-      <c r="B46" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>65</v>
       </c>
-      <c r="B47" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="B52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>67</v>
       </c>
-      <c r="B48" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>68</v>
       </c>
-      <c r="B49" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>69</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B55" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>70</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B56" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>73</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B57" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>74</v>
       </c>
-      <c r="B53" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="B58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>76</v>
       </c>
-      <c r="B54" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>77</v>
       </c>
-      <c r="B55" t="s">
-        <v>13</v>
-      </c>
-      <c r="C55">
+      <c r="B60" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60">
         <v>36</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F60" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>79</v>
       </c>
-      <c r="B56" t="s">
-        <v>13</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B61" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" t="s">
         <v>80</v>
       </c>
-      <c r="E56">
+      <c r="F61">
         <v>1.9</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>81</v>
       </c>
-      <c r="B57" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" t="s">
         <v>80</v>
       </c>
-      <c r="E57" t="b">
+      <c r="F62" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>82</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B63" t="s">
         <v>18</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F63" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>84</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B64" t="s">
         <v>18</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F64" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>83</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B65" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>83</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B66" t="s">
         <v>18</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F66" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>87</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B67" t="s">
         <v>18</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F67" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>88</v>
       </c>
-      <c r="B63" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63">
+      <c r="B68" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>89</v>
       </c>
-      <c r="B64" t="s">
-        <v>13</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B69" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" t="s">
         <v>90</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F69" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>92</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B70" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>93</v>
       </c>
-      <c r="B66" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B71" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>94</v>
       </c>
-      <c r="B67" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="B72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>95</v>
       </c>
-      <c r="B68" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="B73" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>96</v>
       </c>
-      <c r="B69" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="B74" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>97</v>
       </c>
-      <c r="B70" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="B75" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>98</v>
       </c>
-      <c r="B71" t="s">
-        <v>13</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="B76" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>100</v>
       </c>
-      <c r="B72" t="s">
-        <v>13</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="B77" t="s">
+        <v>13</v>
+      </c>
+      <c r="F77" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>102</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B78" t="s">
         <v>103</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F78" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>105</v>
       </c>
-      <c r="B74" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="B79" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>106</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B80" t="s">
         <v>103</v>
       </c>
-      <c r="E75" t="s">
+      <c r="F80" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>108</v>
       </c>
-      <c r="B76" t="s">
-        <v>13</v>
-      </c>
-      <c r="C76">
+      <c r="B81" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81">
         <v>174</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F81" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>109</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B82" t="s">
         <v>110</v>
       </c>
-      <c r="C77">
+      <c r="C82">
         <v>105</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F82" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>112</v>
       </c>
-      <c r="B78" t="s">
-        <v>13</v>
-      </c>
-      <c r="C78">
+      <c r="B83" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83">
         <v>170</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F83" t="s">
         <v>114</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I83" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>117</v>
       </c>
-      <c r="B79" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="B84" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>119</v>
       </c>
-      <c r="B80" t="s">
-        <v>8</v>
-      </c>
-      <c r="E80" t="s">
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="F85" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>121</v>
       </c>
-      <c r="B81" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>122</v>
       </c>
-      <c r="B82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>123</v>
       </c>
-      <c r="B83" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>124</v>
       </c>
-      <c r="B84" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>125</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B90" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F90" xr:uid="{85E9EE67-5E71-8E4C-BE9F-30F08F868F8E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Extra comments on the dmpt spreadsheets
</commit_message>
<xml_diff>
--- a/doc/crosswalk_rdmp.xlsx
+++ b/doc/crosswalk_rdmp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Desktop/Provisioner/rb2-migrate/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19C99C4-AC33-0649-BAB3-674ACF2190A3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137B16BF-0156-7241-B420-D799462541C7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34340" yWindow="-3580" windowWidth="29300" windowHeight="16540" xr2:uid="{D40799DA-BD77-124F-A81D-CFE600731E6F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{D40799DA-BD77-124F-A81D-CFE600731E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="203">
   <si>
     <t xml:space="preserve">Field </t>
   </si>
@@ -516,9 +516,6 @@
     <t>some blanks and one unmapped</t>
   </si>
   <si>
-    <t>Have mapped these but check blanks</t>
-  </si>
-  <si>
     <t>Present in the 9 mystery records (see below)</t>
   </si>
   <si>
@@ -597,9 +594,6 @@
     <t>seo_codes</t>
   </si>
   <si>
-    <t>not in new RDMP</t>
-  </si>
-  <si>
     <t>disposal_date</t>
   </si>
   <si>
@@ -625,6 +619,24 @@
   </si>
   <si>
     <t>retention_period_justification</t>
+  </si>
+  <si>
+    <t>dc_identifier</t>
+  </si>
+  <si>
+    <t>dc_title</t>
+  </si>
+  <si>
+    <t>givenname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>familyname</t>
+  </si>
+  <si>
+    <t>map to new dc:rightsHolder_dc:name</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0153FD-7F44-7F45-A0A3-8BCD7A703616}">
   <dimension ref="A1:J105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68:XFD68"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1308,10 +1320,10 @@
         <v>15</v>
       </c>
       <c r="E19" t="s">
+        <v>182</v>
+      </c>
+      <c r="G19" t="s">
         <v>183</v>
-      </c>
-      <c r="G19" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1339,7 +1351,7 @@
         <v>40</v>
       </c>
       <c r="E21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1350,7 +1362,7 @@
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G22" t="s">
         <v>32</v>
@@ -1374,6 +1386,12 @@
       <c r="B24" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C24" s="1">
+        <v>84</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -1383,7 +1401,7 @@
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G25" t="s">
         <v>151</v>
@@ -1397,7 +1415,7 @@
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G26" t="s">
         <v>151</v>
@@ -1499,6 +1517,9 @@
       <c r="B34" t="s">
         <v>123</v>
       </c>
+      <c r="D34" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -1507,6 +1528,9 @@
       <c r="B35" t="s">
         <v>123</v>
       </c>
+      <c r="D35" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
@@ -1515,6 +1539,9 @@
       <c r="B36" t="s">
         <v>123</v>
       </c>
+      <c r="D36" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1523,6 +1550,9 @@
       <c r="B37" t="s">
         <v>123</v>
       </c>
+      <c r="D37" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -1531,6 +1561,9 @@
       <c r="B38" t="s">
         <v>123</v>
       </c>
+      <c r="D38" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -1556,6 +1589,9 @@
       <c r="B40" t="s">
         <v>123</v>
       </c>
+      <c r="D40" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -1564,6 +1600,9 @@
       <c r="B41" t="s">
         <v>123</v>
       </c>
+      <c r="D41" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -1572,6 +1611,9 @@
       <c r="B42" t="s">
         <v>123</v>
       </c>
+      <c r="D42" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -1580,6 +1622,9 @@
       <c r="B43" t="s">
         <v>123</v>
       </c>
+      <c r="D43" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -1588,6 +1633,9 @@
       <c r="B44" t="s">
         <v>123</v>
       </c>
+      <c r="D44" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -1613,6 +1661,9 @@
       <c r="B46" t="s">
         <v>123</v>
       </c>
+      <c r="D46" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -1621,6 +1672,9 @@
       <c r="B47" t="s">
         <v>123</v>
       </c>
+      <c r="D47" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -1629,6 +1683,9 @@
       <c r="B48" t="s">
         <v>123</v>
       </c>
+      <c r="D48" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -1637,6 +1694,9 @@
       <c r="B49" t="s">
         <v>123</v>
       </c>
+      <c r="D49" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -1645,6 +1705,9 @@
       <c r="B50" t="s">
         <v>123</v>
       </c>
+      <c r="D50" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
@@ -1743,10 +1806,10 @@
         <v>36</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>189</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -1788,7 +1851,7 @@
         <v>160</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>161</v>
@@ -1813,10 +1876,7 @@
         <v>17</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1841,7 +1901,7 @@
         <v>9</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -1873,6 +1933,9 @@
       <c r="B71" t="s">
         <v>123</v>
       </c>
+      <c r="D71" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -1881,6 +1944,9 @@
       <c r="B72" t="s">
         <v>123</v>
       </c>
+      <c r="D72" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -1889,6 +1955,9 @@
       <c r="B73" t="s">
         <v>123</v>
       </c>
+      <c r="D73" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -1897,6 +1966,9 @@
       <c r="B74" t="s">
         <v>123</v>
       </c>
+      <c r="D74" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -1905,6 +1977,9 @@
       <c r="B75" t="s">
         <v>123</v>
       </c>
+      <c r="D75" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
@@ -1917,7 +1992,7 @@
         <v>93</v>
       </c>
       <c r="H76" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1961,10 +2036,10 @@
         <v>49</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G80" s="1" t="s">
         <v>101</v>
@@ -1992,7 +2067,7 @@
         <v>105</v>
       </c>
       <c r="E82" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2003,7 +2078,7 @@
         <v>53</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>101</v>
@@ -2011,13 +2086,13 @@
     </row>
     <row r="84" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>106</v>
@@ -2034,7 +2109,7 @@
         <v>8</v>
       </c>
       <c r="E85" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
@@ -2045,7 +2120,7 @@
         <v>8</v>
       </c>
       <c r="E86" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G86" t="s">
         <v>112</v>
@@ -2059,7 +2134,7 @@
         <v>8</v>
       </c>
       <c r="E87" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
@@ -2070,7 +2145,7 @@
         <v>8</v>
       </c>
       <c r="E88" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
@@ -2081,7 +2156,7 @@
         <v>8</v>
       </c>
       <c r="E89" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
@@ -2092,7 +2167,7 @@
         <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
@@ -2103,60 +2178,60 @@
         <v>8</v>
       </c>
       <c r="E91" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="97" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="101" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="102" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="103" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="104" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added handler functions for FORs, SEOs and people. Not working for some roles (collaborator and supervisor)
</commit_message>
<xml_diff>
--- a/doc/crosswalk_rdmp.xlsx
+++ b/doc/crosswalk_rdmp.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Desktop/Provisioner/rb2-migrate/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137B16BF-0156-7241-B420-D799462541C7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4177C11-10EF-A548-9FF9-2C319B234114}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{D40799DA-BD77-124F-A81D-CFE600731E6F}"/>
+    <workbookView xWindow="-33300" yWindow="380" windowWidth="28800" windowHeight="16060" xr2:uid="{D40799DA-BD77-124F-A81D-CFE600731E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$91</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="209">
   <si>
     <t xml:space="preserve">Field </t>
   </si>
@@ -637,6 +637,24 @@
   </si>
   <si>
     <t>map to new dc:rightsHolder_dc:name</t>
+  </si>
+  <si>
+    <t>Rb2 web check</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>handler</t>
+  </si>
+  <si>
+    <t>handler fired but not in interface</t>
+  </si>
+  <si>
+    <t>handler working</t>
+  </si>
+  <si>
+    <t>handler was not being triggered</t>
   </si>
 </sst>
 </file>
@@ -1022,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0153FD-7F44-7F45-A0A3-8BCD7A703616}">
-  <dimension ref="A1:J105"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1033,10 +1051,10 @@
     <col min="1" max="1" width="48.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="39.83203125" customWidth="1"/>
-    <col min="5" max="6" width="25.1640625" customWidth="1"/>
+    <col min="5" max="7" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1056,10 +1074,13 @@
         <v>137</v>
       </c>
       <c r="G1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1067,7 +1088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1083,11 +1104,11 @@
       <c r="E3" t="s">
         <v>108</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1104,7 +1125,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1121,7 +1142,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1138,7 +1159,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1148,11 +1169,11 @@
       <c r="C7" s="2">
         <v>191</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -1162,11 +1183,11 @@
       <c r="D8" t="s">
         <v>134</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1183,18 +1204,18 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1211,7 +1232,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1225,7 +1246,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1239,7 +1260,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1274,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1267,7 +1288,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1277,11 +1298,11 @@
       <c r="C16" s="1">
         <v>12</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1291,11 +1312,11 @@
       <c r="C17" s="1">
         <v>2</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1305,11 +1326,11 @@
       <c r="C18" s="2">
         <v>12</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1322,11 +1343,11 @@
       <c r="E19" t="s">
         <v>182</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1336,11 +1357,11 @@
       <c r="C20" s="1">
         <v>32</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1354,7 +1375,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1364,22 +1385,22 @@
       <c r="E22" t="s">
         <v>184</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
@@ -1389,50 +1410,56 @@
       <c r="C24" s="1">
         <v>84</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>205</v>
       </c>
       <c r="E25" t="s">
         <v>186</v>
       </c>
       <c r="G25" t="s">
+        <v>204</v>
+      </c>
+      <c r="H25" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>37</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>205</v>
       </c>
       <c r="E26" t="s">
         <v>187</v>
       </c>
       <c r="G26" t="s">
+        <v>204</v>
+      </c>
+      <c r="H26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
@@ -1443,7 +1470,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -1453,11 +1480,11 @@
       <c r="C29" s="2">
         <v>127</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1471,7 +1498,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1484,11 +1511,11 @@
       <c r="E31" t="s">
         <v>153</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1496,7 +1523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -1509,8 +1536,11 @@
       <c r="E33" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>118</v>
       </c>
@@ -1521,7 +1551,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>119</v>
       </c>
@@ -1532,7 +1562,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>120</v>
       </c>
@@ -1543,7 +1573,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -1554,7 +1584,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>122</v>
       </c>
@@ -1565,7 +1595,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>46</v>
       </c>
@@ -1581,8 +1611,11 @@
       <c r="E39" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G39" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1593,7 +1626,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -1604,7 +1637,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -1615,7 +1648,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -1626,7 +1659,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -1637,7 +1670,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -1653,8 +1686,11 @@
       <c r="E45" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G45" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -1665,7 +1701,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1676,7 +1712,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -1687,7 +1723,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -1698,7 +1734,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -1709,18 +1745,18 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="H51" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>60</v>
       </c>
@@ -1728,7 +1764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>61</v>
       </c>
@@ -1736,7 +1772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>63</v>
       </c>
@@ -1744,7 +1780,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>64</v>
       </c>
@@ -1752,7 +1788,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -1760,7 +1796,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -1768,7 +1804,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>69</v>
       </c>
@@ -1776,18 +1812,18 @@
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>70</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -1795,7 +1831,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
@@ -1808,11 +1844,11 @@
       <c r="E61" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="H61" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -1822,11 +1858,11 @@
       <c r="C62" t="s">
         <v>75</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>1.9</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -1836,11 +1872,11 @@
       <c r="C63" t="s">
         <v>75</v>
       </c>
-      <c r="G63" t="b">
+      <c r="H63" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>77</v>
       </c>
@@ -1853,22 +1889,22 @@
       <c r="E64" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G64" s="1" t="s">
+      <c r="H64" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="H65" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>78</v>
       </c>
@@ -1879,18 +1915,18 @@
         <v>196</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="H67" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>82</v>
       </c>
@@ -1900,11 +1936,11 @@
       <c r="C68" s="1">
         <v>9</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="H68" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>83</v>
       </c>
@@ -1914,19 +1950,22 @@
       <c r="C69" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G69" s="4" t="s">
+      <c r="H69" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>86</v>
       </c>
       <c r="B70" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>87</v>
       </c>
@@ -1937,7 +1976,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>88</v>
       </c>
@@ -1948,7 +1987,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>89</v>
       </c>
@@ -1959,7 +1998,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -1970,7 +2009,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>91</v>
       </c>
@@ -1981,43 +2020,43 @@
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="H76" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="H77" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>96</v>
       </c>
       <c r="B78" t="s">
         <v>97</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="79" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>99</v>
       </c>
@@ -2025,7 +2064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>100</v>
       </c>
@@ -2041,22 +2080,22 @@
       <c r="E80" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="G80" s="1" t="s">
+      <c r="H80" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G81" s="3" t="s">
+      <c r="H81" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>103</v>
       </c>
@@ -2070,7 +2109,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>104</v>
       </c>
@@ -2080,11 +2119,11 @@
       <c r="D83" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="G83" s="1" t="s">
+      <c r="H83" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>176</v>
       </c>
@@ -2094,14 +2133,14 @@
       <c r="E84" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="G84" s="3" t="s">
+      <c r="H84" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="J84" s="3" t="s">
+      <c r="K84" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>109</v>
       </c>
@@ -2112,7 +2151,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>111</v>
       </c>
@@ -2122,11 +2161,11 @@
       <c r="E86" t="s">
         <v>189</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>113</v>
       </c>
@@ -2137,7 +2176,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>114</v>
       </c>
@@ -2148,7 +2187,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>115</v>
       </c>
@@ -2159,7 +2198,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>116</v>
       </c>
@@ -2170,7 +2209,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>117</v>
       </c>
@@ -2181,7 +2220,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>172</v>
       </c>
@@ -2235,7 +2274,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G91" xr:uid="{85E9EE67-5E71-8E4C-BE9F-30F08F868F8E}"/>
+  <autoFilter ref="A1:H91" xr:uid="{85E9EE67-5E71-8E4C-BE9F-30F08F868F8E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved the outdir behaviour - now creates two subdirectories, originals/ and new/, to dump before and after JSON
</commit_message>
<xml_diff>
--- a/doc/crosswalk_rdmp.xlsx
+++ b/doc/crosswalk_rdmp.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Desktop/Provisioner/rb2-migrate/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4177C11-10EF-A548-9FF9-2C319B234114}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15B8F3C-3126-AB40-9810-AAF4BBDB0021}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33300" yWindow="380" windowWidth="28800" windowHeight="16060" xr2:uid="{D40799DA-BD77-124F-A81D-CFE600731E6F}"/>
+    <workbookView xWindow="1660" yWindow="460" windowWidth="26040" windowHeight="16000" xr2:uid="{D40799DA-BD77-124F-A81D-CFE600731E6F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$92</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="221">
   <si>
     <t xml:space="preserve">Field </t>
   </si>
@@ -655,6 +655,42 @@
   </si>
   <si>
     <t>handler was not being triggered</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Json format check</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>dataowner_email</t>
+  </si>
+  <si>
+    <t>[ ] not [ "" ]</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>not in rb2</t>
+  </si>
+  <si>
+    <t>ok but get rid of nulls</t>
+  </si>
+  <si>
+    <t>is "as" in migrated records</t>
+  </si>
+  <si>
+    <t>n - AS</t>
+  </si>
+  <si>
+    <t>n - A</t>
+  </si>
+  <si>
+    <t>in rb2, is full label</t>
   </si>
 </sst>
 </file>
@@ -1040,21 +1076,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA0153FD-7F44-7F45-A0A3-8BCD7A703616}">
-  <dimension ref="A1:K105"/>
+  <dimension ref="A1:L106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" customWidth="1"/>
+    <col min="1" max="1" width="66.5" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="39.83203125" customWidth="1"/>
     <col min="5" max="7" width="25.1640625" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1071,16 +1108,19 @@
         <v>107</v>
       </c>
       <c r="F1" t="s">
+        <v>210</v>
+      </c>
+      <c r="G1" t="s">
         <v>137</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>203</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1088,7 +1128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1104,11 +1144,14 @@
       <c r="E3" t="s">
         <v>108</v>
       </c>
-      <c r="H3" t="s">
+      <c r="F3" t="s">
+        <v>209</v>
+      </c>
+      <c r="I3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1124,8 +1167,11 @@
       <c r="E4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1141,8 +1187,11 @@
       <c r="E5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1158,8 +1207,11 @@
       <c r="E6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1169,11 +1221,14 @@
       <c r="C7" s="2">
         <v>191</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="F7" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>132</v>
       </c>
@@ -1183,296 +1238,350 @@
       <c r="D8" t="s">
         <v>134</v>
       </c>
-      <c r="H8" t="s">
+      <c r="F8" t="s">
+        <v>211</v>
+      </c>
+      <c r="I8" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>136</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
+        <v>209</v>
+      </c>
+      <c r="G10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11">
-        <v>206</v>
-      </c>
-      <c r="D11" t="s">
-        <v>141</v>
-      </c>
-      <c r="E11" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>18</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
+      <c r="C12">
+        <v>206</v>
+      </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="F12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+      <c r="F13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
         <v>140</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="F15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>21</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>21</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E16" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="F16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1">
-        <v>12</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1">
+        <v>12</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
         <v>2</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="F18" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="2">
-        <v>12</v>
-      </c>
-      <c r="H18" s="2" t="s">
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2">
+        <v>12</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>8</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>15</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>182</v>
       </c>
-      <c r="H19" t="s">
+      <c r="F20" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I20" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1">
         <v>32</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="F21" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>40</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="F22" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>8</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>184</v>
       </c>
-      <c r="H22" t="s">
+      <c r="F23" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1">
         <v>84</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="F25" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>36</v>
-      </c>
-      <c r="B25" t="s">
-        <v>205</v>
-      </c>
-      <c r="E25" t="s">
-        <v>186</v>
-      </c>
-      <c r="G25" t="s">
-        <v>204</v>
-      </c>
-      <c r="H25" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>37</v>
       </c>
       <c r="B26" t="s">
         <v>205</v>
       </c>
       <c r="E26" t="s">
+        <v>186</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H26" t="s">
+        <v>204</v>
+      </c>
+      <c r="I26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>205</v>
+      </c>
+      <c r="E27" t="s">
         <v>187</v>
       </c>
-      <c r="G26" t="s">
+      <c r="F27" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H27" t="s">
         <v>204</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I27" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="F28" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I28" s="2" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="2">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>12</v>
@@ -1480,391 +1589,409 @@
       <c r="C29" s="2">
         <v>127</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="F29" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2">
+        <v>127</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>42</v>
-      </c>
-      <c r="B30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" t="s">
-        <v>92</v>
-      </c>
-      <c r="E30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>43</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
       <c r="D31" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" t="s">
+        <v>140</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="E31" t="s">
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
         <v>153</v>
       </c>
-      <c r="H31" t="s">
+      <c r="F32" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="I32" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>44</v>
       </c>
-      <c r="B32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>47</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>8</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>154</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>154</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H34" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>118</v>
-      </c>
-      <c r="B34" t="s">
-        <v>123</v>
-      </c>
-      <c r="D34" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>119</v>
       </c>
       <c r="B35" t="s">
         <v>123</v>
       </c>
       <c r="D35" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B36" t="s">
         <v>123</v>
       </c>
       <c r="D36" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B37" t="s">
         <v>123</v>
       </c>
       <c r="D37" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B38" t="s">
         <v>123</v>
       </c>
       <c r="D38" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>46</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>48</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>155</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>156</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E40" t="s">
         <v>157</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H40" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>45</v>
-      </c>
-      <c r="B40" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>49</v>
       </c>
       <c r="B41" t="s">
         <v>123</v>
       </c>
       <c r="D41" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
         <v>123</v>
       </c>
       <c r="D42" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" t="s">
         <v>123</v>
       </c>
       <c r="D43" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B44" t="s">
         <v>123</v>
       </c>
       <c r="D44" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>53</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>48</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>155</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>158</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>159</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H46" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>54</v>
-      </c>
-      <c r="B46" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>55</v>
       </c>
       <c r="B47" t="s">
         <v>123</v>
       </c>
       <c r="D47" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
         <v>123</v>
       </c>
       <c r="D48" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
         <v>123</v>
       </c>
       <c r="D49" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B50" t="s">
         <v>123</v>
       </c>
       <c r="D50" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H51" s="2" t="s">
+      <c r="B52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B52" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
+      <c r="B53" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B54" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B55" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B56" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>65</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>66</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>69</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>70</v>
       </c>
-      <c r="B59" t="s">
-        <v>12</v>
-      </c>
-      <c r="H59" t="s">
+      <c r="B60" t="s">
+        <v>12</v>
+      </c>
+      <c r="I60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>72</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
+      <c r="F61" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C61" s="1">
+      <c r="B62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="1">
         <v>36</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H61" s="1" t="s">
+      <c r="F62" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I62" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>74</v>
-      </c>
-      <c r="B62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C62" t="s">
-        <v>75</v>
-      </c>
-      <c r="H62">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>76</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
@@ -1872,409 +1999,477 @@
       <c r="C63" t="s">
         <v>75</v>
       </c>
-      <c r="H63" t="b">
+      <c r="I63">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64" t="s">
+        <v>12</v>
+      </c>
+      <c r="C64" t="s">
+        <v>75</v>
+      </c>
+      <c r="I64" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+    <row r="65" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E64" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="H64" s="1" t="s">
+      <c r="F65" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="F66" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I66" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1" t="s">
+    <row r="67" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
+      <c r="F67" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="F68" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I68" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
+    <row r="69" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C68" s="1">
+      <c r="B69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="1">
         <v>9</v>
       </c>
-      <c r="H68" s="1" t="s">
+      <c r="I69" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+    <row r="70" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C69" s="4" t="s">
+      <c r="B70" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H69" s="4" t="s">
+      <c r="I70" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>86</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>48</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H71" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>87</v>
-      </c>
-      <c r="B71" t="s">
-        <v>123</v>
-      </c>
-      <c r="D71" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>88</v>
       </c>
       <c r="B72" t="s">
         <v>123</v>
       </c>
       <c r="D72" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B73" t="s">
         <v>123</v>
       </c>
       <c r="D73" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
         <v>123</v>
       </c>
       <c r="D74" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
         <v>123</v>
       </c>
       <c r="D75" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>91</v>
+      </c>
+      <c r="B76" t="s">
+        <v>123</v>
+      </c>
+      <c r="D76" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="76" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
+    <row r="77" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B76" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H76" s="2" t="s">
+      <c r="B77" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I77" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="J77" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
+    <row r="78" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B77" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H77" s="2" t="s">
+      <c r="B78" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I78" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>96</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B79" t="s">
         <v>97</v>
       </c>
-      <c r="H78" t="s">
+      <c r="F79" t="s">
+        <v>209</v>
+      </c>
+      <c r="I79" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="79" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
+    <row r="80" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B79" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1" t="s">
+      <c r="B80" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B81" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C81" s="1">
         <v>49</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="H80" s="1" t="s">
+      <c r="F81" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I81" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="81" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+    <row r="82" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H81" s="3" t="s">
+      <c r="B82" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="I82" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>103</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>30</v>
       </c>
-      <c r="C82">
+      <c r="C83">
         <v>105</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E83" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1" t="s">
+      <c r="F83" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C83" s="1">
+      <c r="C84" s="1">
         <v>53</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="H83" s="1" t="s">
+      <c r="F84" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I84" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+    <row r="85" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B84" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E84" s="3" t="s">
+      <c r="B85" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="H84" s="3" t="s">
+      <c r="F85" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="I85" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K84" s="3" t="s">
+      <c r="L85" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>109</v>
-      </c>
-      <c r="B85" t="s">
-        <v>8</v>
-      </c>
-      <c r="E85" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>111</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
       </c>
       <c r="E86" t="s">
-        <v>189</v>
-      </c>
-      <c r="H86" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+      <c r="F86" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B87" t="s">
         <v>8</v>
       </c>
       <c r="E87" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+      <c r="F87" t="s">
+        <v>219</v>
+      </c>
+      <c r="I87" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B88" t="s">
         <v>8</v>
       </c>
       <c r="E88" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+      <c r="F88" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B89" t="s">
         <v>8</v>
       </c>
       <c r="E89" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+      <c r="F89" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B90" t="s">
         <v>8</v>
       </c>
       <c r="E90" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+      <c r="F90" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B91" t="s">
         <v>8</v>
       </c>
       <c r="E91" t="s">
+        <v>193</v>
+      </c>
+      <c r="F91" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>117</v>
+      </c>
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="E92" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="F92" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>172</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="102" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="103" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="104" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>171</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H91" xr:uid="{85E9EE67-5E71-8E4C-BE9F-30F08F868F8E}"/>
+  <autoFilter ref="A1:I92" xr:uid="{85E9EE67-5E71-8E4C-BE9F-30F08F868F8E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>